<commit_message>
added new PROFILES for comparison with Obs.
</commit_message>
<xml_diff>
--- a/Observations/Resulting_SWI_Observations.xlsx
+++ b/Observations/Resulting_SWI_Observations.xlsx
@@ -31,493 +31,493 @@
     <t>4298m</t>
   </si>
   <si>
-    <t>       Fswi_TOC</t>
-  </si>
-  <si>
-    <t> -6.1151e-04</t>
-  </si>
-  <si>
-    <t> -7.5193e-04</t>
-  </si>
-  <si>
-    <t> -3.0900e-05</t>
-  </si>
-  <si>
-    <t> -2.8710e-05</t>
-  </si>
-  <si>
-    <t>      Fswi_TOC1</t>
-  </si>
-  <si>
-    <t> -3.7398e-04</t>
-  </si>
-  <si>
-    <t> -2.7417e-04</t>
-  </si>
-  <si>
-    <t> -2.2895e-05</t>
-  </si>
-  <si>
-    <t> -2.6380e-05</t>
-  </si>
-  <si>
-    <t>      Fswi_TOC2</t>
-  </si>
-  <si>
-    <t> -2.3754e-04</t>
-  </si>
-  <si>
-    <t> -4.7776e-04</t>
-  </si>
-  <si>
-    <t> -8.0046e-06</t>
-  </si>
-  <si>
-    <t> -2.3308e-06</t>
-  </si>
-  <si>
-    <t>         F_TOC1</t>
-  </si>
-  <si>
-    <t> -7.1970e-39</t>
-  </si>
-  <si>
-    <t> -1.2522e-14</t>
-  </si>
-  <si>
-    <t> -1.1839e-44</t>
-  </si>
-  <si>
-    <t> -2.1133e-181</t>
-  </si>
-  <si>
-    <t>         F_TOC2</t>
-  </si>
-  <si>
-    <t> -2.3724e-04</t>
-  </si>
-  <si>
-    <t> -4.3436e-04</t>
-  </si>
-  <si>
-    <t> -5.2832e-06</t>
-  </si>
-  <si>
-    <t> -2.1426e-06</t>
-  </si>
-  <si>
-    <t>          F_TOC</t>
-  </si>
-  <si>
-    <t>            zox</t>
-  </si>
-  <si>
-    <t>            zxf</t>
-  </si>
-  <si>
-    <t>            rO2</t>
-  </si>
-  <si>
-    <t> [1x1 struct]</t>
-  </si>
-  <si>
-    <t>         flxzox</t>
-  </si>
-  <si>
-    <t> -1.9152e-04</t>
-  </si>
-  <si>
-    <t> -8.4895e-05</t>
-  </si>
-  <si>
-    <t> -3.7001e-06</t>
-  </si>
-  <si>
-    <t> -2.7620e-06</t>
-  </si>
-  <si>
-    <t>        conczox</t>
-  </si>
-  <si>
-    <t> 8.4568e-17</t>
-  </si>
-  <si>
-    <t> 2.4991e-16</t>
-  </si>
-  <si>
-    <t> -2.8376e-19</t>
-  </si>
-  <si>
-    <t> 7.9130e-18</t>
-  </si>
-  <si>
-    <t>       flxswiO2</t>
-  </si>
-  <si>
-    <t> -3.5665e-04</t>
-  </si>
-  <si>
-    <t> -8.2759e-05</t>
-  </si>
-  <si>
-    <t> -3.7791e-05</t>
-  </si>
-  <si>
-    <t> -3.9880e-05</t>
-  </si>
-  <si>
-    <t>           zno3</t>
-  </si>
-  <si>
-    <t>           rNO3</t>
-  </si>
-  <si>
-    <t>        flxzno3</t>
-  </si>
-  <si>
-    <t> 9.3973e-14</t>
-  </si>
-  <si>
-    <t> 9.4865e-17</t>
-  </si>
-  <si>
-    <t> 5.7347e-20</t>
-  </si>
-  <si>
-    <t> -2.8371e-21</t>
-  </si>
-  <si>
-    <t>       conczno3</t>
-  </si>
-  <si>
-    <t> 6.3209e-17</t>
-  </si>
-  <si>
-    <t> -3.6538e-17</t>
-  </si>
-  <si>
-    <t> 1.6094e-20</t>
-  </si>
-  <si>
-    <t> -5.8276e-19</t>
-  </si>
-  <si>
-    <t>      flxswiNO3</t>
-  </si>
-  <si>
-    <t> 2.1344e-06</t>
-  </si>
-  <si>
-    <t> -2.7819e-05</t>
-  </si>
-  <si>
-    <t> 1.6437e-06</t>
-  </si>
-  <si>
-    <t> 8.8665e-07</t>
-  </si>
-  <si>
-    <t>           zso4</t>
-  </si>
-  <si>
-    <t>           rSO4</t>
-  </si>
-  <si>
-    <t>        flxzso4</t>
-  </si>
-  <si>
-    <t>       conczso4</t>
-  </si>
-  <si>
-    <t> 2.7568e-05</t>
-  </si>
-  <si>
-    <t> 2.3529e-05</t>
-  </si>
-  <si>
-    <t> 2.7847e-05</t>
-  </si>
-  <si>
-    <t> 2.7992e-05</t>
-  </si>
-  <si>
-    <t>      flxswiSO4</t>
-  </si>
-  <si>
-    <t> -4.5019e-05</t>
-  </si>
-  <si>
-    <t> -1.3562e-04</t>
-  </si>
-  <si>
-    <t> -8.9863e-08</t>
-  </si>
-  <si>
-    <t> -3.2917e-09</t>
-  </si>
-  <si>
-    <t>    conczinfNH4</t>
-  </si>
-  <si>
-    <t> 1.0238e-07</t>
-  </si>
-  <si>
-    <t> 1.0140e-06</t>
-  </si>
-  <si>
-    <t> 3.8382e-08</t>
-  </si>
-  <si>
-    <t> 4.2871e-09</t>
-  </si>
-  <si>
-    <t>      flxswiNH4</t>
-  </si>
-  <si>
-    <t> 5.8811e-06</t>
-  </si>
-  <si>
-    <t> 1.3938e-05</t>
-  </si>
-  <si>
-    <t> 1.5981e-07</t>
-  </si>
-  <si>
-    <t> 1.5707e-07</t>
-  </si>
-  <si>
-    <t>           rNH4</t>
-  </si>
-  <si>
-    <t>    conczinfH2S</t>
-  </si>
-  <si>
-    <t> 4.3225e-07</t>
-  </si>
-  <si>
-    <t> 4.4706e-06</t>
-  </si>
-  <si>
-    <t> 1.5344e-07</t>
-  </si>
-  <si>
-    <t> 7.7762e-09</t>
-  </si>
-  <si>
-    <t>      flxswiH2S</t>
-  </si>
-  <si>
-    <t> 4.5019e-05</t>
-  </si>
-  <si>
-    <t> 1.3562e-04</t>
-  </si>
-  <si>
-    <t> 8.9863e-08</t>
-  </si>
-  <si>
-    <t> 3.2917e-09</t>
-  </si>
-  <si>
-    <t>           rH2S</t>
-  </si>
-  <si>
-    <t>    conczinfPO4</t>
-  </si>
-  <si>
-    <t> 1.5007e-08</t>
-  </si>
-  <si>
-    <t> 9.0924e-08</t>
-  </si>
-  <si>
-    <t> 5.0502e-09</t>
-  </si>
-  <si>
-    <t> 5.0040e-09</t>
-  </si>
-  <si>
-    <t>       flxswi_P</t>
-  </si>
-  <si>
-    <t> 2.0100e-08</t>
-  </si>
-  <si>
-    <t> 2.7494e-08</t>
-  </si>
-  <si>
-    <t> 1.1844e-09</t>
-  </si>
-  <si>
-    <t> 1.2344e-09</t>
-  </si>
-  <si>
-    <t>       flxswi_M</t>
-  </si>
-  <si>
-    <t> 5.2360e-11</t>
-  </si>
-  <si>
-    <t> 2.1349e-09</t>
-  </si>
-  <si>
-    <t> 1.3460e-08</t>
-  </si>
-  <si>
-    <t> 1.9267e-08</t>
-  </si>
-  <si>
-    <t>         rPO4_M</t>
-  </si>
-  <si>
-    <t>    conczinfDIC</t>
-  </si>
-  <si>
-    <t> 3.2932e-06</t>
-  </si>
-  <si>
-    <t> 8.9072e-06</t>
-  </si>
-  <si>
-    <t> 2.4633e-06</t>
-  </si>
-  <si>
-    <t> 2.6191e-06</t>
-  </si>
-  <si>
-    <t>      flxswiDIC</t>
-  </si>
-  <si>
-    <t> 3.7427e-04</t>
-  </si>
-  <si>
-    <t> 3.1757e-04</t>
-  </si>
-  <si>
-    <t> 2.5616e-05</t>
-  </si>
-  <si>
-    <t> 2.6565e-05</t>
-  </si>
-  <si>
-    <t>           rDIC</t>
-  </si>
-  <si>
-    <t>    conczinfALK</t>
-  </si>
-  <si>
-    <t> 3.1187e-06</t>
-  </si>
-  <si>
-    <t> 1.0277e-05</t>
-  </si>
-  <si>
-    <t> 2.6609e-06</t>
-  </si>
-  <si>
-    <t> 2.4195e-06</t>
-  </si>
-  <si>
-    <t>      flxswiALK</t>
-  </si>
-  <si>
-    <t> 2.0997e-05</t>
-  </si>
-  <si>
-    <t> 2.4653e-04</t>
-  </si>
-  <si>
-    <t> -5.2905e-06</t>
-  </si>
-  <si>
-    <t> -4.5727e-06</t>
-  </si>
-  <si>
-    <t>           rALK</t>
-  </si>
-  <si>
-    <t>frac1 concentration at zinf 2.04767e-72 </t>
-  </si>
-  <si>
-    <t>frac1 concentration at zinf 9.07816e-24 </t>
-  </si>
-  <si>
-    <t>frac1 concentration at zinf 8.55949e-88 </t>
-  </si>
-  <si>
-    <t>frac1 concentration at zinf 0 </t>
-  </si>
-  <si>
-    <t>frac2 concentration at zinf 0.00389041 </t>
-  </si>
-  <si>
-    <t>frac2 concentration at zinf 0.00626823 </t>
-  </si>
-  <si>
-    <t>frac2 concentration at zinf 0.000484013 </t>
-  </si>
-  <si>
-    <t>frac2 concentration at zinf 0.00221154 </t>
-  </si>
-  <si>
-    <t>both concentration at zinf 0.00389041 </t>
-  </si>
-  <si>
-    <t>both concentration at zinf 0.00626823 </t>
-  </si>
-  <si>
-    <t>both concentration at zinf 0.000484013 </t>
-  </si>
-  <si>
-    <t>both concentration at zinf 0.00221154 </t>
-  </si>
-  <si>
-    <t>frac1 concentration at swi 0.00572 </t>
-  </si>
-  <si>
-    <t>frac1 concentration at swi 0.00433333 </t>
-  </si>
-  <si>
-    <t>frac1 concentration at swi 0.000975 </t>
-  </si>
-  <si>
-    <t>frac1 concentration at swi 0.00179833 </t>
-  </si>
-  <si>
-    <t>frac2 concentration at swi 0.0039 </t>
-  </si>
-  <si>
-    <t>frac2 concentration at swi 0.00758333 </t>
-  </si>
-  <si>
-    <t>frac2 concentration at swi 0.00108333 </t>
-  </si>
-  <si>
-    <t>frac2 concentration at swi 0.0026 </t>
-  </si>
-  <si>
-    <t>both concentration at swi 0.00962 </t>
-  </si>
-  <si>
-    <t>both concentration at swi 0.0119167 </t>
-  </si>
-  <si>
-    <t>both concentration at swi 0.00205833 </t>
-  </si>
-  <si>
-    <t>both concentration at swi 0.00439833 </t>
-  </si>
-  <si>
-    <t>sed preservation of POC 0.404409 </t>
-  </si>
-  <si>
-    <t>sed preservation of POC 0.526005 </t>
-  </si>
-  <si>
-    <t>sed preservation of POC 0.235148 </t>
-  </si>
-  <si>
-    <t>sed preservation of POC 0.502813 </t>
+    <t>Fswi_TOC</t>
+  </si>
+  <si>
+    <t>-6.1151e-04</t>
+  </si>
+  <si>
+    <t>-7.5193e-04</t>
+  </si>
+  <si>
+    <t>-3.0900e-05</t>
+  </si>
+  <si>
+    <t>-2.8710e-05</t>
+  </si>
+  <si>
+    <t>Fswi_TOC1</t>
+  </si>
+  <si>
+    <t>-3.7398e-04</t>
+  </si>
+  <si>
+    <t>-2.7417e-04</t>
+  </si>
+  <si>
+    <t>-2.2895e-05</t>
+  </si>
+  <si>
+    <t>-2.6380e-05</t>
+  </si>
+  <si>
+    <t>Fswi_TOC2</t>
+  </si>
+  <si>
+    <t>-2.3754e-04</t>
+  </si>
+  <si>
+    <t>-4.7776e-04</t>
+  </si>
+  <si>
+    <t>-8.0046e-06</t>
+  </si>
+  <si>
+    <t>-2.3308e-06</t>
+  </si>
+  <si>
+    <t>F_TOC1</t>
+  </si>
+  <si>
+    <t>-7.1970e-39</t>
+  </si>
+  <si>
+    <t>-1.2522e-14</t>
+  </si>
+  <si>
+    <t>-1.1839e-44</t>
+  </si>
+  <si>
+    <t>-2.1133e-181</t>
+  </si>
+  <si>
+    <t>F_TOC2</t>
+  </si>
+  <si>
+    <t>-2.3724e-04</t>
+  </si>
+  <si>
+    <t>-4.3436e-04</t>
+  </si>
+  <si>
+    <t>-5.2832e-06</t>
+  </si>
+  <si>
+    <t>-2.1426e-06</t>
+  </si>
+  <si>
+    <t>F_TOC</t>
+  </si>
+  <si>
+    <t>zox</t>
+  </si>
+  <si>
+    <t>zxf</t>
+  </si>
+  <si>
+    <t>rO2</t>
+  </si>
+  <si>
+    <t>[1x1 struct]</t>
+  </si>
+  <si>
+    <t>flxzox</t>
+  </si>
+  <si>
+    <t>-1.9152e-04</t>
+  </si>
+  <si>
+    <t>-8.4895e-05</t>
+  </si>
+  <si>
+    <t>-3.7001e-06</t>
+  </si>
+  <si>
+    <t>-2.7620e-06</t>
+  </si>
+  <si>
+    <t>conczox</t>
+  </si>
+  <si>
+    <t>8.4568e-17</t>
+  </si>
+  <si>
+    <t>2.4991e-16</t>
+  </si>
+  <si>
+    <t>-2.8376e-19</t>
+  </si>
+  <si>
+    <t>7.9130e-18</t>
+  </si>
+  <si>
+    <t>flxswiO2</t>
+  </si>
+  <si>
+    <t>-3.5665e-04</t>
+  </si>
+  <si>
+    <t>-8.2759e-05</t>
+  </si>
+  <si>
+    <t>-3.7791e-05</t>
+  </si>
+  <si>
+    <t>-3.9880e-05</t>
+  </si>
+  <si>
+    <t>zno3</t>
+  </si>
+  <si>
+    <t>rNO3</t>
+  </si>
+  <si>
+    <t>flxzno3</t>
+  </si>
+  <si>
+    <t>9.3973e-14</t>
+  </si>
+  <si>
+    <t>9.4865e-17</t>
+  </si>
+  <si>
+    <t>5.7347e-20</t>
+  </si>
+  <si>
+    <t>-2.8371e-21</t>
+  </si>
+  <si>
+    <t>conczno3</t>
+  </si>
+  <si>
+    <t>6.3209e-17</t>
+  </si>
+  <si>
+    <t>-3.6538e-17</t>
+  </si>
+  <si>
+    <t>1.6094e-20</t>
+  </si>
+  <si>
+    <t>-5.8276e-19</t>
+  </si>
+  <si>
+    <t>flxswiNO3</t>
+  </si>
+  <si>
+    <t>2.1344e-06</t>
+  </si>
+  <si>
+    <t>-2.7819e-05</t>
+  </si>
+  <si>
+    <t>1.6437e-06</t>
+  </si>
+  <si>
+    <t>8.8665e-07</t>
+  </si>
+  <si>
+    <t>zso4</t>
+  </si>
+  <si>
+    <t>rSO4</t>
+  </si>
+  <si>
+    <t>flxzso4</t>
+  </si>
+  <si>
+    <t>conczso4</t>
+  </si>
+  <si>
+    <t>2.7568e-05</t>
+  </si>
+  <si>
+    <t>2.3529e-05</t>
+  </si>
+  <si>
+    <t>2.7847e-05</t>
+  </si>
+  <si>
+    <t>2.7992e-05</t>
+  </si>
+  <si>
+    <t>flxswiSO4</t>
+  </si>
+  <si>
+    <t>-4.5019e-05</t>
+  </si>
+  <si>
+    <t>-1.3562e-04</t>
+  </si>
+  <si>
+    <t>-8.9863e-08</t>
+  </si>
+  <si>
+    <t>-3.2917e-09</t>
+  </si>
+  <si>
+    <t>conczinfNH4</t>
+  </si>
+  <si>
+    <t>1.0238e-07</t>
+  </si>
+  <si>
+    <t>1.0140e-06</t>
+  </si>
+  <si>
+    <t>3.8382e-08</t>
+  </si>
+  <si>
+    <t>4.2871e-09</t>
+  </si>
+  <si>
+    <t>flxswiNH4</t>
+  </si>
+  <si>
+    <t>5.8811e-06</t>
+  </si>
+  <si>
+    <t>1.3938e-05</t>
+  </si>
+  <si>
+    <t>1.5981e-07</t>
+  </si>
+  <si>
+    <t>1.5707e-07</t>
+  </si>
+  <si>
+    <t>rNH4</t>
+  </si>
+  <si>
+    <t>conczinfH2S</t>
+  </si>
+  <si>
+    <t>4.3225e-07</t>
+  </si>
+  <si>
+    <t>4.4706e-06</t>
+  </si>
+  <si>
+    <t>1.5344e-07</t>
+  </si>
+  <si>
+    <t>7.7762e-09</t>
+  </si>
+  <si>
+    <t>flxswiH2S</t>
+  </si>
+  <si>
+    <t>4.5019e-05</t>
+  </si>
+  <si>
+    <t>1.3562e-04</t>
+  </si>
+  <si>
+    <t>8.9863e-08</t>
+  </si>
+  <si>
+    <t>3.2917e-09</t>
+  </si>
+  <si>
+    <t>rH2S</t>
+  </si>
+  <si>
+    <t>conczinfPO4</t>
+  </si>
+  <si>
+    <t>1.5007e-08</t>
+  </si>
+  <si>
+    <t>9.0924e-08</t>
+  </si>
+  <si>
+    <t>5.0502e-09</t>
+  </si>
+  <si>
+    <t>5.0040e-09</t>
+  </si>
+  <si>
+    <t>flxswi_P</t>
+  </si>
+  <si>
+    <t>2.0100e-08</t>
+  </si>
+  <si>
+    <t>2.7494e-08</t>
+  </si>
+  <si>
+    <t>1.1844e-09</t>
+  </si>
+  <si>
+    <t>1.2344e-09</t>
+  </si>
+  <si>
+    <t>flxswi_M</t>
+  </si>
+  <si>
+    <t>5.2360e-11</t>
+  </si>
+  <si>
+    <t>2.1349e-09</t>
+  </si>
+  <si>
+    <t>1.3460e-08</t>
+  </si>
+  <si>
+    <t>1.9267e-08</t>
+  </si>
+  <si>
+    <t>rPO4_M</t>
+  </si>
+  <si>
+    <t>conczinfDIC</t>
+  </si>
+  <si>
+    <t>3.2932e-06</t>
+  </si>
+  <si>
+    <t>9.3072e-06</t>
+  </si>
+  <si>
+    <t>2.4633e-06</t>
+  </si>
+  <si>
+    <t>2.6191e-06</t>
+  </si>
+  <si>
+    <t>flxswiDIC</t>
+  </si>
+  <si>
+    <t>3.7427e-04</t>
+  </si>
+  <si>
+    <t>3.1757e-04</t>
+  </si>
+  <si>
+    <t>2.5616e-05</t>
+  </si>
+  <si>
+    <t>2.6565e-05</t>
+  </si>
+  <si>
+    <t>rDIC</t>
+  </si>
+  <si>
+    <t>conczinfALK</t>
+  </si>
+  <si>
+    <t>3.1187e-06</t>
+  </si>
+  <si>
+    <t>1.0277e-05</t>
+  </si>
+  <si>
+    <t>2.6609e-06</t>
+  </si>
+  <si>
+    <t>2.4195e-06</t>
+  </si>
+  <si>
+    <t>flxswiALK</t>
+  </si>
+  <si>
+    <t>2.0997e-05</t>
+  </si>
+  <si>
+    <t>2.4653e-04</t>
+  </si>
+  <si>
+    <t>-5.2905e-06</t>
+  </si>
+  <si>
+    <t>-4.5727e-06</t>
+  </si>
+  <si>
+    <t>rALK</t>
+  </si>
+  <si>
+    <t>frac1 concentration at zinf 2.04767e-72</t>
+  </si>
+  <si>
+    <t>frac1 concentration at zinf 9.07816e-24</t>
+  </si>
+  <si>
+    <t>frac1 concentration at zinf 8.55949e-88</t>
+  </si>
+  <si>
+    <t>frac1 concentration at zinf 0</t>
+  </si>
+  <si>
+    <t>frac2 concentration at zinf 0.00389041</t>
+  </si>
+  <si>
+    <t>frac2 concentration at zinf 0.00626823</t>
+  </si>
+  <si>
+    <t>frac2 concentration at zinf 0.000484013</t>
+  </si>
+  <si>
+    <t>frac2 concentration at zinf 0.00221154</t>
+  </si>
+  <si>
+    <t>both concentration at zinf 0.00389041</t>
+  </si>
+  <si>
+    <t>both concentration at zinf 0.00626823</t>
+  </si>
+  <si>
+    <t>both concentration at zinf 0.000484013</t>
+  </si>
+  <si>
+    <t>both concentration at zinf 0.00221154</t>
+  </si>
+  <si>
+    <t>frac1 concentration at swi 0.00572</t>
+  </si>
+  <si>
+    <t>frac1 concentration at swi 0.00433333</t>
+  </si>
+  <si>
+    <t>frac1 concentration at swi 0.000975</t>
+  </si>
+  <si>
+    <t>frac1 concentration at swi 0.00179833</t>
+  </si>
+  <si>
+    <t>frac2 concentration at swi 0.0039</t>
+  </si>
+  <si>
+    <t>frac2 concentration at swi 0.00758333</t>
+  </si>
+  <si>
+    <t>frac2 concentration at swi 0.00108333</t>
+  </si>
+  <si>
+    <t>frac2 concentration at swi 0.0026</t>
+  </si>
+  <si>
+    <t>both concentration at swi 0.00962</t>
+  </si>
+  <si>
+    <t>both concentration at swi 0.0119167</t>
+  </si>
+  <si>
+    <t>both concentration at swi 0.00205833</t>
+  </si>
+  <si>
+    <t>both concentration at swi 0.00439833</t>
+  </si>
+  <si>
+    <t>sed preservation of POC 0.404409</t>
+  </si>
+  <si>
+    <t>sed preservation of POC 0.526005</t>
+  </si>
+  <si>
+    <t>sed preservation of POC 0.235148</t>
+  </si>
+  <si>
+    <t>sed preservation of POC 0.502813</t>
   </si>
 </sst>
 </file>
@@ -531,6 +531,7 @@
   <fonts count="5">
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -551,6 +552,7 @@
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
       <sz val="14"/>
@@ -622,16 +624,16 @@
   <dimension ref="A1:N48"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="O3" activeCellId="0" pane="topLeft" sqref="O3"/>
+      <selection activeCell="F26" activeCellId="0" pane="topLeft" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="11.5764705882353"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.8196078431373"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.8980392156863"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.9" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -645,7 +647,7 @@
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
         <v>4</v>
       </c>
@@ -671,7 +673,7 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
         <v>9</v>
       </c>
@@ -697,7 +699,7 @@
         <v>13</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
         <v>14</v>
       </c>
@@ -723,7 +725,7 @@
         <v>18</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
         <v>19</v>
       </c>
@@ -749,7 +751,7 @@
         <v>23</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
         <v>24</v>
       </c>
@@ -775,7 +777,7 @@
         <v>28</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="8">
       <c r="A8" s="0" t="s">
         <v>29</v>
       </c>
@@ -801,7 +803,7 @@
         <v>28</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
         <v>30</v>
       </c>
@@ -827,7 +829,7 @@
         <v>3.4892</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="10">
       <c r="A10" s="0" t="s">
         <v>31</v>
       </c>
@@ -853,7 +855,7 @@
         <v>0.9721</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="11">
       <c r="A11" s="0" t="s">
         <v>32</v>
       </c>
@@ -879,7 +881,7 @@
         <v>33</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="12">
       <c r="A12" s="0" t="s">
         <v>34</v>
       </c>
@@ -905,7 +907,7 @@
         <v>38</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="13">
       <c r="A13" s="0" t="s">
         <v>39</v>
       </c>
@@ -931,7 +933,7 @@
         <v>43</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="14">
       <c r="A14" s="0" t="s">
         <v>44</v>
       </c>
@@ -957,7 +959,7 @@
         <v>48</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="15">
       <c r="A15" s="0" t="s">
         <v>49</v>
       </c>
@@ -983,7 +985,7 @@
         <v>31.9522</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="16">
       <c r="A16" s="0" t="s">
         <v>50</v>
       </c>
@@ -1009,7 +1011,7 @@
         <v>33</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="17">
       <c r="A17" s="0" t="s">
         <v>51</v>
       </c>
@@ -1035,7 +1037,7 @@
         <v>55</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="18">
       <c r="A18" s="0" t="s">
         <v>56</v>
       </c>
@@ -1061,7 +1063,7 @@
         <v>60</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="19">
       <c r="A19" s="0" t="s">
         <v>61</v>
       </c>
@@ -1087,7 +1089,7 @@
         <v>65</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="20">
       <c r="A20" s="0" t="s">
         <v>66</v>
       </c>
@@ -1113,7 +1115,7 @@
         <v>50</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="21">
       <c r="A21" s="0" t="s">
         <v>67</v>
       </c>
@@ -1139,7 +1141,7 @@
         <v>33</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="22">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="22">
       <c r="A22" s="0" t="s">
         <v>68</v>
       </c>
@@ -1165,7 +1167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="23">
       <c r="A23" s="0" t="s">
         <v>69</v>
       </c>
@@ -1191,7 +1193,7 @@
         <v>73</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="24">
       <c r="A24" s="0" t="s">
         <v>74</v>
       </c>
@@ -1217,7 +1219,7 @@
         <v>78</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="25">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="25">
       <c r="A25" s="0" t="s">
         <v>79</v>
       </c>
@@ -1243,7 +1245,7 @@
         <v>83</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="26">
       <c r="A26" s="0" t="s">
         <v>84</v>
       </c>
@@ -1269,7 +1271,7 @@
         <v>88</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="27">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="27">
       <c r="A27" s="0" t="s">
         <v>89</v>
       </c>
@@ -1295,7 +1297,7 @@
         <v>33</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="28">
       <c r="A28" s="0" t="s">
         <v>90</v>
       </c>
@@ -1321,7 +1323,7 @@
         <v>94</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="29">
       <c r="A29" s="0" t="s">
         <v>95</v>
       </c>
@@ -1347,7 +1349,7 @@
         <v>99</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="30">
       <c r="A30" s="0" t="s">
         <v>100</v>
       </c>
@@ -1373,7 +1375,7 @@
         <v>33</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="31">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="31">
       <c r="A31" s="0" t="s">
         <v>101</v>
       </c>
@@ -1399,7 +1401,7 @@
         <v>105</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="32">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="32">
       <c r="A32" s="0" t="s">
         <v>106</v>
       </c>
@@ -1425,7 +1427,7 @@
         <v>110</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="33">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="33">
       <c r="A33" s="0" t="s">
         <v>111</v>
       </c>
@@ -1451,7 +1453,7 @@
         <v>115</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="34">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="34">
       <c r="A34" s="0" t="s">
         <v>116</v>
       </c>
@@ -1477,7 +1479,7 @@
         <v>33</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="35">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="35">
       <c r="A35" s="0" t="s">
         <v>117</v>
       </c>
@@ -1503,7 +1505,7 @@
         <v>121</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="36">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="36">
       <c r="A36" s="0" t="s">
         <v>122</v>
       </c>
@@ -1529,7 +1531,7 @@
         <v>126</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="37">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="37">
       <c r="A37" s="0" t="s">
         <v>127</v>
       </c>
@@ -1555,7 +1557,7 @@
         <v>33</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="38">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="38">
       <c r="A38" s="0" t="s">
         <v>128</v>
       </c>
@@ -1581,7 +1583,7 @@
         <v>132</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="39">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="39">
       <c r="A39" s="0" t="s">
         <v>133</v>
       </c>
@@ -1607,7 +1609,7 @@
         <v>137</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="40">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="40">
       <c r="A40" s="0" t="s">
         <v>138</v>
       </c>
@@ -1633,8 +1635,8 @@
         <v>33</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="41"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="42">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="41"/>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="42">
       <c r="A42" s="0" t="s">
         <v>139</v>
       </c>
@@ -1648,7 +1650,7 @@
         <v>142</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="43">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="43">
       <c r="A43" s="0" t="s">
         <v>143</v>
       </c>
@@ -1662,7 +1664,7 @@
         <v>146</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="44">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="44">
       <c r="A44" s="0" t="s">
         <v>147</v>
       </c>
@@ -1676,7 +1678,7 @@
         <v>150</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="45">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="45">
       <c r="A45" s="0" t="s">
         <v>151</v>
       </c>
@@ -1690,7 +1692,7 @@
         <v>154</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="46">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="46">
       <c r="A46" s="0" t="s">
         <v>155</v>
       </c>
@@ -1704,7 +1706,7 @@
         <v>158</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="47">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="47">
       <c r="A47" s="0" t="s">
         <v>159</v>
       </c>
@@ -1718,7 +1720,7 @@
         <v>162</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="48">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="48">
       <c r="A48" s="0" t="s">
         <v>163</v>
       </c>
@@ -1750,17 +1752,17 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1775,17 +1777,17 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>